<commit_message>
Update: alternate api for way id searching
</commit_message>
<xml_diff>
--- a/Mapping/unimelb_southbank_url.xlsx
+++ b/Mapping/unimelb_southbank_url.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/boat_amorntiyanggoon_unimelb_edu_au/Documents/Casual Tasks/URL_extraction/mapping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HYC-MacBookPro/Documents/Digital Estate/hyperlink-pasting/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_33E9C3E815FB0C81319372EBF9E1717A6C26BAC5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{138BD228-29BA-41CF-9C25-CD792648E613}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB5A8BC-17B3-7143-B96C-6F3C9269B202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>SOUTHBANK THE HUB</t>
   </si>
   <si>
-    <t>SOUTHBANK PERFORMING ARTS, ST KILDA RD</t>
-  </si>
-  <si>
     <t>SOUTHBANK OLD POLICE HOSPITAL</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>STURT ST SERVICE CENTRE / ART STUDIO 3</t>
   </si>
   <si>
-    <t>SOUTHBANK PERFORMING ARTS, DODDS ST</t>
-  </si>
-  <si>
     <t>SOUTHBANK MELBOURNE THEATRE COMPANY</t>
   </si>
   <si>
@@ -200,6 +194,12 @@
   </si>
   <si>
     <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=877</t>
+  </si>
+  <si>
+    <t>SOUTHBANK PERFORMING ARTS - ST KILDA RD</t>
+  </si>
+  <si>
+    <t>SOUTHBANK PERFORMING ARTS - DODDS ST</t>
   </si>
 </sst>
 </file>
@@ -617,15 +617,15 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,213 +636,213 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the building name to match with SISfm
</commit_message>
<xml_diff>
--- a/Mapping/unimelb_southbank_url.xlsx
+++ b/Mapping/unimelb_southbank_url.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HYC-MacBookPro/Documents/Digital Estate/hyperlink-pasting/Mapping/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB5A8BC-17B3-7143-B96C-6F3C9269B202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,6 +40,9 @@
     <t>SOUTHBANK THE HUB</t>
   </si>
   <si>
+    <t>SOUTHBANK PERFORMING ARTS, ST KILDA RD</t>
+  </si>
+  <si>
     <t>SOUTHBANK OLD POLICE HOSPITAL</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
     <t>STURT ST SERVICE CENTRE / ART STUDIO 3</t>
   </si>
   <si>
+    <t>SOUTHBANK PERFORMING ARTS, DODDS ST</t>
+  </si>
+  <si>
     <t>SOUTHBANK MELBOURNE THEATRE COMPANY</t>
   </si>
   <si>
@@ -139,74 +139,68 @@
     <t>877</t>
   </si>
   <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=298</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=860</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=861</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=862</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=863</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=864</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=865</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=868</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=871</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=872</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=873</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=874</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=875</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=876</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=879</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=887</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=867</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=880</t>
-  </si>
-  <si>
-    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=877</t>
-  </si>
-  <si>
-    <t>SOUTHBANK PERFORMING ARTS - ST KILDA RD</t>
-  </si>
-  <si>
-    <t>SOUTHBANK PERFORMING ARTS - DODDS ST</t>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 298 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 860  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 861 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 862 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 863 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 864  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 865 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 868  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 871 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 872  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 873 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 874 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 875  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 876 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 879 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 887 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 867 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 880 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 877 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,14 +276,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -336,7 +322,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,27 +354,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,24 +388,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -613,19 +563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,236 +581,236 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C11" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
+    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C15" r:id="rId14"/>
+    <hyperlink ref="C16" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
+    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C19" r:id="rId18"/>
+    <hyperlink ref="C20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update the col name for STH
</commit_message>
<xml_diff>
--- a/Mapping/unimelb_southbank_url.xlsx
+++ b/Mapping/unimelb_southbank_url.xlsx
@@ -1,28 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/boat_amorntiyanggoon_unimelb_edu_au/Documents/Casual Tasks/URL_extraction/mapping/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_17E141E61D7B4E846F9272CD19DB00045926BC3B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEA6F823-BE39-4722-8A7C-65A824EE1670}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
-    <t>Building name</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>url</t>
+    <t>building_name</t>
+  </si>
+  <si>
+    <t>building_no</t>
+  </si>
+  <si>
+    <t>website:map</t>
   </si>
   <si>
     <t>SOUTHBANK MELBOURNE THEATRE COMPANY - HQ</t>
@@ -199,8 +205,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +282,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -322,7 +336,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -354,9 +368,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,6 +420,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -563,14 +613,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -592,7 +645,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -603,7 +656,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -614,7 +667,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -625,7 +678,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -636,7 +689,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -647,7 +700,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -658,7 +711,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -669,7 +722,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -680,7 +733,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -691,7 +744,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -702,7 +755,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -713,7 +766,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -724,7 +777,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -735,7 +788,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -746,7 +799,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -757,7 +810,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -768,7 +821,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -779,7 +832,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -792,25 +845,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C15" r:id="rId14"/>
-    <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="C17" r:id="rId16"/>
-    <hyperlink ref="C18" r:id="rId17"/>
-    <hyperlink ref="C19" r:id="rId18"/>
-    <hyperlink ref="C20" r:id="rId19"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove the space on building no at url
</commit_message>
<xml_diff>
--- a/Mapping/unimelb_southbank_url.xlsx
+++ b/Mapping/unimelb_southbank_url.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/boat_amorntiyanggoon_unimelb_edu_au/Documents/Casual Tasks/URL_extraction/mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_17E141E61D7B4E846F9272CD19DB00045926BC3B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEA6F823-BE39-4722-8A7C-65A824EE1670}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_33E9C3E815FB0C813193721419E24F44714CBACD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0AC551D-21C8-4016-8901-BDCFF5F4C73B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <t>building_name</t>
   </si>
   <si>
-    <t>building_no</t>
+    <t>No</t>
   </si>
   <si>
     <t>website:map</t>
@@ -145,61 +145,61 @@
     <t>877</t>
   </si>
   <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 298 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 860  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 861 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 862 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 863 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 864  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 865 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 868  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 871 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 872  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 873 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 874 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 875  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 876 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 879 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 887 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 867 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 880 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi= 877 </t>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=298</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=860</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=861</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=862</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=863</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=864</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=865</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=868</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=871</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=872</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=873</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=874</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=875</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=876</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=879</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=887</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=867</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=880</t>
+  </si>
+  <si>
+    <t>https://use.mazemap.com/?campusid=216&amp;sharepoitype=identifier&amp;sharepoi=877</t>
   </si>
 </sst>
 </file>
@@ -616,12 +616,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>